<commit_message>
Previous experimental results are included
</commit_message>
<xml_diff>
--- a/auxiliary/test_sets.xlsx
+++ b/auxiliary/test_sets.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22905"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\41395550350ana\Desktop\aliyurekli\github\RecSys-MPD\auxiliary\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14685"/>
   </bookViews>
   <sheets>
     <sheet name="research" sheetId="2" r:id="rId1"/>
@@ -12,18 +17,18 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>CATEGORY NO</t>
   </si>
@@ -112,25 +117,34 @@
     <t>100K</t>
   </si>
   <si>
-    <t>10 folds, each having 10000 playlists. Constructed using only category 1.</t>
-  </si>
-  <si>
     <t>1M</t>
   </si>
   <si>
-    <t>10 folds, each having 100000 playlists. Constructed using only category 1.</t>
-  </si>
-  <si>
     <t>10fold_100K_a</t>
   </si>
   <si>
     <t>10fold_1M_a</t>
+  </si>
+  <si>
+    <t>10 folds, each having 10000 playlists. 
+Includes categories 1, 2, 3.</t>
+  </si>
+  <si>
+    <t>10 folds, each having 10000 playlists. 
+Includes only category 1.</t>
+  </si>
+  <si>
+    <t>10 folds, each having 100000 playlists. 
+Includes only category 1.</t>
+  </si>
+  <si>
+    <t>10fold_100K_b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -205,21 +219,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="İzlenen Köprü" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="İzlenen Köprü" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="İzlenen Köprü" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Köprü" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Köprü" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Köprü" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -490,7 +507,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -498,23 +515,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.5703125" customWidth="1"/>
     <col min="6" max="7" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -531,9 +548,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>28</v>
@@ -544,25 +561,42 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2">
         <v>10</v>
       </c>
       <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>31</v>
+      <c r="E4" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -584,20 +618,20 @@
       <selection sqref="A1:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
-    <col min="8" max="8" width="18.5" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -626,7 +660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -655,7 +689,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -684,7 +718,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -713,7 +747,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -742,7 +776,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -771,7 +805,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -800,7 +834,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -829,7 +863,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -858,7 +892,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -887,7 +921,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>

</xml_diff>